<commit_message>
Modifying spreadsheet with query times and memory usage to demonstrate the javaVScpp of CPT/+
</commit_message>
<xml_diff>
--- a/cptVSsd_cpt_done_on_cpp.xlsx
+++ b/cptVSsd_cpt_done_on_cpp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -129,6 +129,33 @@
   </si>
   <si>
     <t>SD_II / CDS</t>
+  </si>
+  <si>
+    <t>Java CPT query time (ms)</t>
+  </si>
+  <si>
+    <t>Java CPT+ query time (ms)</t>
+  </si>
+  <si>
+    <t>cpp CPT query time (ms)</t>
+  </si>
+  <si>
+    <t>cpp CPT+ query time (ms)</t>
+  </si>
+  <si>
+    <t>Java CPT memory (MB)*</t>
+  </si>
+  <si>
+    <t>*As reported with calculations</t>
+  </si>
+  <si>
+    <t>Java CPT+ memory (MB)*</t>
+  </si>
+  <si>
+    <t>cpp CPT memory (MB)*</t>
+  </si>
+  <si>
+    <t>cpp CPT+ memory (MB)*</t>
   </si>
 </sst>
 </file>
@@ -537,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,9 +586,18 @@
     <col min="16" max="17" width="30.1640625" customWidth="1"/>
     <col min="18" max="18" width="26" customWidth="1"/>
     <col min="19" max="19" width="23.5" customWidth="1"/>
+    <col min="20" max="20" width="30.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.1640625" customWidth="1"/>
+    <col min="22" max="22" width="22.1640625" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" customWidth="1"/>
+    <col min="24" max="24" width="24.83203125" customWidth="1"/>
+    <col min="25" max="25" width="26.1640625" customWidth="1"/>
+    <col min="26" max="26" width="29.6640625" customWidth="1"/>
+    <col min="27" max="27" width="28.6640625" customWidth="1"/>
+    <col min="28" max="28" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,8 +655,32 @@
       <c r="S1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -680,7 +740,7 @@
         <v>1.5992988553964163</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -740,7 +800,7 @@
         <v>0.86660083187478787</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -800,7 +860,7 @@
         <v>0.83706418024162821</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -860,7 +920,7 @@
         <v>1.1045662405605889</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -920,7 +980,7 @@
         <v>0.80720064225282528</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -980,7 +1040,7 @@
         <v>0.8506838501631947</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1040,7 +1100,7 @@
         <v>1.1702174253089317</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1160,7 @@
         <v>0.96062842722425668</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1160,7 +1220,7 @@
         <v>1.2324857857233245</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1280,7 @@
         <v>1.1970549468592131</v>
       </c>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:20" x14ac:dyDescent="0.2">
       <c r="H18" t="s">
         <v>24</v>
       </c>
@@ -1237,7 +1297,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:20" x14ac:dyDescent="0.2">
       <c r="H19" s="3">
         <f>O2/F2</f>
         <v>2.0429124999999999</v>
@@ -1247,11 +1307,11 @@
         <v>40.962125</v>
       </c>
       <c r="J19" s="3">
-        <f>(M2+L2+I2+G2)/F2</f>
+        <f t="shared" ref="J19:J28" si="1">(M2+L2+I2+G2)/F2</f>
         <v>37.9605125</v>
       </c>
       <c r="K19" s="3">
-        <f>I19/H19</f>
+        <f t="shared" ref="K19:K28" si="2">I19/H19</f>
         <v>20.050846524263768</v>
       </c>
       <c r="M19" s="3">
@@ -1262,254 +1322,257 @@
         <f>H2/F2</f>
         <v>1.4551812500000001</v>
       </c>
-    </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="T19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20" x14ac:dyDescent="0.2">
       <c r="H20" s="3">
-        <f t="shared" ref="H20:H28" si="1">O3/F3</f>
+        <f t="shared" ref="H20:H28" si="3">O3/F3</f>
         <v>2.8483000000000001</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20:I28" si="2">N3/F3</f>
+        <f t="shared" ref="I20:I28" si="4">N3/F3</f>
         <v>84.671800000000005</v>
       </c>
       <c r="J20" s="3">
-        <f>(M3+L3+I3+G3)/F3</f>
+        <f t="shared" si="1"/>
         <v>80.335667999999998</v>
       </c>
       <c r="K20" s="3">
-        <f>I20/H20</f>
+        <f t="shared" si="2"/>
         <v>29.727135484323984</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" ref="M20:M28" si="3">G3/F3</f>
+        <f t="shared" ref="M20:M28" si="5">G3/F3</f>
         <v>64.876199999999997</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" ref="N20:N28" si="4">H3/F3</f>
+        <f t="shared" ref="N20:N28" si="6">H3/F3</f>
         <v>1.967584</v>
       </c>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:20" x14ac:dyDescent="0.2">
       <c r="H21" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8972105263157899</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="4"/>
+        <v>179.27807017543861</v>
+      </c>
+      <c r="J21" s="3">
         <f t="shared" si="1"/>
-        <v>3.8972105263157899</v>
-      </c>
-      <c r="I21" s="3">
+        <v>174.81260526315791</v>
+      </c>
+      <c r="K21" s="3">
         <f t="shared" si="2"/>
-        <v>179.27807017543861</v>
-      </c>
-      <c r="J21" s="3">
-        <f>(M4+L4+I4+G4)/F4</f>
-        <v>174.81260526315791</v>
-      </c>
-      <c r="K21" s="3">
-        <f>I21/H21</f>
         <v>46.001638598907903</v>
       </c>
       <c r="M21" s="3">
+        <f t="shared" si="5"/>
+        <v>162.63070175438597</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="6"/>
+        <v>2.8912719298245619</v>
+      </c>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H22" s="3">
         <f t="shared" si="3"/>
-        <v>162.63070175438597</v>
-      </c>
-      <c r="N21" s="3">
+        <v>3.3000500000000001</v>
+      </c>
+      <c r="I22" s="3">
         <f t="shared" si="4"/>
-        <v>2.8912719298245619</v>
-      </c>
-      <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H22" s="3">
+        <v>37.733249999999998</v>
+      </c>
+      <c r="J22" s="3">
         <f t="shared" si="1"/>
-        <v>3.3000500000000001</v>
-      </c>
-      <c r="I22" s="3">
+        <v>26.818075</v>
+      </c>
+      <c r="K22" s="3">
         <f t="shared" si="2"/>
-        <v>37.733249999999998</v>
-      </c>
-      <c r="J22" s="3">
-        <f>(M5+L5+I5+G5)/F5</f>
-        <v>26.818075</v>
-      </c>
-      <c r="K22" s="3">
-        <f>I22/H22</f>
         <v>11.434144937197921</v>
       </c>
       <c r="M22" s="3">
+        <f t="shared" si="5"/>
+        <v>0.748</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="6"/>
+        <v>1.9905249999999999</v>
+      </c>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H23" s="3">
         <f t="shared" si="3"/>
-        <v>0.748</v>
-      </c>
-      <c r="N22" s="3">
+        <v>2.5869870129870129</v>
+      </c>
+      <c r="I23" s="3">
         <f t="shared" si="4"/>
-        <v>1.9905249999999999</v>
-      </c>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H23" s="3">
+        <v>58.575324675324673</v>
+      </c>
+      <c r="J23" s="3">
         <f t="shared" si="1"/>
-        <v>2.5869870129870129</v>
-      </c>
-      <c r="I23" s="3">
+        <v>53.223318181818179</v>
+      </c>
+      <c r="K23" s="3">
         <f t="shared" si="2"/>
-        <v>58.575324675324673</v>
-      </c>
-      <c r="J23" s="3">
-        <f>(M6+L6+I6+G6)/F6</f>
-        <v>53.223318181818179</v>
-      </c>
-      <c r="K23" s="3">
-        <f>I23/H23</f>
         <v>22.642295605377562</v>
       </c>
       <c r="M23" s="3">
+        <f t="shared" si="5"/>
+        <v>41.248441558441556</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="6"/>
+        <v>1.6301558441558441</v>
+      </c>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H24" s="3">
         <f t="shared" si="3"/>
-        <v>41.248441558441556</v>
-      </c>
-      <c r="N23" s="3">
+        <v>4.7269142857142858</v>
+      </c>
+      <c r="I24" s="3">
         <f t="shared" si="4"/>
-        <v>1.6301558441558441</v>
-      </c>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H24" s="3">
+        <v>40.462000000000003</v>
+      </c>
+      <c r="J24" s="3">
         <f t="shared" si="1"/>
-        <v>4.7269142857142858</v>
-      </c>
-      <c r="I24" s="3">
+        <v>34.517428571428574</v>
+      </c>
+      <c r="K24" s="3">
         <f t="shared" si="2"/>
-        <v>40.462000000000003</v>
-      </c>
-      <c r="J24" s="3">
-        <f>(M7+L7+I7+G7)/F7</f>
-        <v>34.517428571428574</v>
-      </c>
-      <c r="K24" s="3">
-        <f>I24/H24</f>
         <v>8.5599182795178983</v>
       </c>
       <c r="M24" s="3">
+        <f t="shared" si="5"/>
+        <v>19.390914285714285</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="6"/>
+        <v>3.4960285714285719</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H25" s="3">
         <f t="shared" si="3"/>
-        <v>19.390914285714285</v>
-      </c>
-      <c r="N24" s="3">
+        <v>1.1779068965517241</v>
+      </c>
+      <c r="I25" s="3">
         <f t="shared" si="4"/>
-        <v>3.4960285714285719</v>
-      </c>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H25" s="3">
+        <v>33.773000000000003</v>
+      </c>
+      <c r="J25" s="3">
         <f t="shared" si="1"/>
-        <v>1.1779068965517241</v>
-      </c>
-      <c r="I25" s="3">
+        <v>15.512727586206898</v>
+      </c>
+      <c r="K25" s="3">
         <f t="shared" si="2"/>
-        <v>33.773000000000003</v>
-      </c>
-      <c r="J25" s="3">
-        <f>(M8+L8+I8+G8)/F8</f>
-        <v>15.512727586206898</v>
-      </c>
-      <c r="K25" s="3">
-        <f>I25/H25</f>
         <v>28.672045387346934</v>
       </c>
       <c r="M25" s="3">
+        <f t="shared" si="5"/>
+        <v>0.23406896551724138</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.50332068965517252</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H26" s="3">
         <f t="shared" si="3"/>
-        <v>0.23406896551724138</v>
-      </c>
-      <c r="N25" s="3">
+        <v>2.1336410256410261</v>
+      </c>
+      <c r="I26" s="3">
         <f t="shared" si="4"/>
-        <v>0.50332068965517252</v>
-      </c>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H26" s="3">
+        <v>29.80769230769231</v>
+      </c>
+      <c r="J26" s="3">
         <f t="shared" si="1"/>
-        <v>2.1336410256410261</v>
-      </c>
-      <c r="I26" s="3">
+        <v>20.326425641025644</v>
+      </c>
+      <c r="K26" s="3">
         <f t="shared" si="2"/>
-        <v>29.80769230769231</v>
-      </c>
-      <c r="J26" s="3">
-        <f>(M9+L9+I9+G9)/F9</f>
-        <v>20.326425641025644</v>
-      </c>
-      <c r="K26" s="3">
-        <f>I26/H26</f>
         <v>13.970340816228427</v>
       </c>
       <c r="M26" s="3">
+        <f t="shared" si="5"/>
+        <v>6.5831282051282054</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="6"/>
+        <v>1.1312478632478633</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H27" s="3">
         <f t="shared" si="3"/>
-        <v>6.5831282051282054</v>
-      </c>
-      <c r="N26" s="3">
+        <v>1.7078266666666666</v>
+      </c>
+      <c r="I27" s="3">
         <f t="shared" si="4"/>
-        <v>1.1312478632478633</v>
-      </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H27" s="3">
+        <v>59.489466666666665</v>
+      </c>
+      <c r="J27" s="3">
         <f t="shared" si="1"/>
-        <v>1.7078266666666666</v>
-      </c>
-      <c r="I27" s="3">
+        <v>56.273183999999993</v>
+      </c>
+      <c r="K27" s="3">
         <f t="shared" si="2"/>
-        <v>59.489466666666665</v>
-      </c>
-      <c r="J27" s="3">
-        <f>(M10+L10+I10+G10)/F10</f>
-        <v>56.273183999999993</v>
-      </c>
-      <c r="K27" s="3">
-        <f>I27/H27</f>
         <v>34.833433525650534</v>
       </c>
       <c r="M27" s="3">
+        <f t="shared" si="5"/>
+        <v>47.48746666666667</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" si="6"/>
+        <v>1.1576773333333332</v>
+      </c>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="8:20" x14ac:dyDescent="0.2">
+      <c r="H28" s="3">
         <f t="shared" si="3"/>
-        <v>47.48746666666667</v>
-      </c>
-      <c r="N27" s="3">
+        <v>1.5511467889908255</v>
+      </c>
+      <c r="I28" s="3">
         <f t="shared" si="4"/>
-        <v>1.1576773333333332</v>
-      </c>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H28" s="3">
+        <v>59.461926605504587</v>
+      </c>
+      <c r="J28" s="3">
         <f t="shared" si="1"/>
-        <v>1.5511467889908255</v>
-      </c>
-      <c r="I28" s="3">
+        <v>55.791211009174312</v>
+      </c>
+      <c r="K28" s="3">
         <f t="shared" si="2"/>
-        <v>59.461926605504587</v>
-      </c>
-      <c r="J28" s="3">
-        <f>(M11+L11+I11+G11)/F11</f>
-        <v>55.791211009174312</v>
-      </c>
-      <c r="K28" s="3">
-        <f>I28/H28</f>
         <v>38.334171225787379</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>47.578256880733946</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99376146788990816</v>
       </c>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="8:20" x14ac:dyDescent="0.2">
       <c r="O29" s="5"/>
     </row>
-    <row r="30" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="8:20" x14ac:dyDescent="0.2">
       <c r="O30" s="5"/>
     </row>
   </sheetData>

</xml_diff>